<commit_message>
Update Excel upload method ( level2 screen )
2단계화면 수정
</commit_message>
<xml_diff>
--- a/master/website/static/datatemplates/manucost.xlsx
+++ b/master/website/static/datatemplates/manucost.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,30 +429,35 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>int(11)</t>
+          <t>varchar(50)</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>varchar(50)</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>int(11)</t>
+          <t>varchar(8)</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>int(11)</t>
+          <t>varchar(50)</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>int(255)</t>
+          <t>int(20)</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
+        <is>
+          <t>varchar(50)</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
         <is>
           <t>varchar(50)</t>
         </is>
@@ -461,37 +466,38 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>(id)입력x</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>co_id</t>
+          <t>사업장ID</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>manucost_ym</t>
+          <t>코스트센터ID</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>cstctr_id</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>itemaccnt_id</t>
-        </is>
-      </c>
+          <t>년월</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>manucost_price</t>
+          <t>금액</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>mngmt_1</t>
+          <t>버젼ID</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>관리항목</t>
         </is>
       </c>
     </row>

</xml_diff>